<commit_message>
Corrijo costo del logger
</commit_message>
<xml_diff>
--- a/Documentación/Factibilidad económica/Factibilidad económica.xlsx
+++ b/Documentación/Factibilidad económica/Factibilidad económica.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Repos\Wet-DryPenguins\Diagramas y Gráficos\Factibilidad económica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Repos\Wet-DryPenguins\Documentación\Factibilidad económica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Costos" sheetId="1" r:id="rId1"/>
@@ -804,7 +804,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
@@ -845,24 +845,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,18 +879,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
@@ -919,6 +889,39 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
@@ -1205,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,25 +1229,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="E1" s="36" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="73"/>
+      <c r="E1" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
-      <c r="K1" s="36" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="70"/>
+      <c r="K1" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="38"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="70"/>
       <c r="R1" t="s">
         <v>78</v>
       </c>
@@ -1253,41 +1256,41 @@
       <c r="A2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="39" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="39" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="44" t="s">
+      <c r="M2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="39" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -1790,11 +1793,11 @@
         <v>0.72077143346631101</v>
       </c>
       <c r="H13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="0"/>
-        <v>0.72077143346631101</v>
+        <v>1.441542866932622</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>28</v>
@@ -1975,7 +1978,7 @@
       <c r="H18" s="13"/>
       <c r="I18" s="19">
         <f>SUM(I3:I17)</f>
-        <v>12.22253596710639</v>
+        <v>12.943307400572701</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>44</v>
@@ -2003,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,12 +2025,12 @@
       <c r="A1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="66"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="76"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2036,16 +2039,16 @@
       <c r="B2">
         <v>700</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="67">
+      <c r="E2" s="66">
         <v>1</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="56">
         <v>2</v>
       </c>
-      <c r="G2" s="68">
+      <c r="G2" s="67">
         <v>3</v>
       </c>
     </row>
@@ -2056,7 +2059,7 @@
       <c r="B3" s="16">
         <v>50</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="60" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="4">
@@ -2067,24 +2070,24 @@
         <f>$B$2</f>
         <v>700</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="58">
         <f>$B$2</f>
         <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="64">
         <f>E3*$B$3</f>
         <v>26250</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="64">
         <f t="shared" ref="F4:G4" si="0">F3*$B$3</f>
         <v>35000</v>
       </c>
-      <c r="G4" s="75">
+      <c r="G4" s="65">
         <f t="shared" si="0"/>
         <v>35000</v>
       </c>
@@ -2094,12 +2097,12 @@
       <c r="A6" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
+      <c r="D6" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="76"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2108,16 +2111,16 @@
       <c r="B7">
         <v>14</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="66">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="56">
         <v>2</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="67">
         <v>3</v>
       </c>
     </row>
@@ -2128,7 +2131,7 @@
       <c r="B8" s="16">
         <v>80</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="60" t="s">
         <v>85</v>
       </c>
       <c r="E8" s="4">
@@ -2139,45 +2142,45 @@
         <f>$B$7</f>
         <v>14</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="58">
         <f>$B$7</f>
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="34"/>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="74">
+      <c r="E9" s="64">
         <f>E8*$B$8</f>
         <v>800</v>
       </c>
-      <c r="F9" s="74">
+      <c r="F9" s="64">
         <f t="shared" ref="F9:G9" si="1">F8*$B$8</f>
         <v>1120</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9" s="65">
         <f t="shared" si="1"/>
         <v>1120</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="72"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="73"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="34"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="47"/>
+      <c r="B13" s="41"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="59"/>
+      <c r="B14" s="53"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="59"/>
+      <c r="B15" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2213,7 +2216,7 @@
       <c r="E1" s="23">
         <v>0</v>
       </c>
-      <c r="F1" s="42">
+      <c r="F1" s="36">
         <v>1</v>
       </c>
       <c r="G1" s="23">
@@ -2222,8 +2225,8 @@
       <c r="H1" s="35">
         <v>3</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2235,21 +2238,21 @@
       <c r="D2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="42">
         <f>-Costos!C13</f>
         <v>-29330.320372727783</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="43">
         <v>0</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="42">
         <v>0</v>
       </c>
-      <c r="H2" s="60">
+      <c r="H2" s="54">
         <v>0</v>
       </c>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2261,18 +2264,18 @@
       <c r="D3" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="44">
         <v>0</v>
       </c>
       <c r="F3" s="3">
         <f>Ingresos!E4+Ingresos!E9</f>
         <v>27050</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="44">
         <f>Ingresos!F4+Ingresos!F9</f>
         <v>36120</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="51">
         <f>Ingresos!G4+Ingresos!G9</f>
         <v>36120</v>
       </c>
@@ -2283,21 +2286,21 @@
       <c r="D4" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="44">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="F4" s="3">
         <f>-Ingresos!E3*Costos!$I$18 - Ingresos!E8*Costos!$O$18</f>
-        <v>-6539.0567424019191</v>
-      </c>
-      <c r="G4" s="50">
+        <v>-6917.4617449717325</v>
+      </c>
+      <c r="G4" s="44">
         <f>-Ingresos!F3*Costos!$I$18 - Ingresos!F8*Costos!$O$18</f>
-        <v>-8726.8906805139632</v>
-      </c>
-      <c r="H4" s="57">
+        <v>-9231.4306839403798</v>
+      </c>
+      <c r="H4" s="51">
         <f>-Ingresos!G3*Costos!$I$18 - Ingresos!G8*Costos!$O$18</f>
-        <v>-8726.8906805139632</v>
+        <v>-9231.4306839403798</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -2306,28 +2309,28 @@
       <c r="A5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="41">
         <f>SUM(E9:H9)</f>
-        <v>11057.442994955107</v>
+        <v>10313.153424486163</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="44">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="F5" s="3">
         <f>F3+F4</f>
-        <v>20510.943257598083</v>
-      </c>
-      <c r="G5" s="50">
+        <v>20132.538255028267</v>
+      </c>
+      <c r="G5" s="44">
         <f t="shared" ref="G5:H5" si="0">G3+G4</f>
-        <v>27393.109319486037</v>
-      </c>
-      <c r="H5" s="57">
+        <v>26888.56931605962</v>
+      </c>
+      <c r="H5" s="51">
         <f t="shared" si="0"/>
-        <v>27393.109319486037</v>
+        <v>26888.56931605962</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -2336,27 +2339,27 @@
       <c r="A6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="53">
         <f>IRR(E8:H8)</f>
-        <v>0.42958408895653122</v>
+        <v>0.41542743559083228</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="44">
         <v>0</v>
       </c>
       <c r="F6" s="3">
         <f>-$B$2*F5</f>
-        <v>-4307.298084095597</v>
-      </c>
-      <c r="G6" s="50">
+        <v>-4227.8330335559358</v>
+      </c>
+      <c r="G6" s="44">
         <f>-$B$2*G5</f>
-        <v>-5752.5529570920671</v>
-      </c>
-      <c r="H6" s="57">
+        <v>-5646.5995563725201</v>
+      </c>
+      <c r="H6" s="51">
         <f>-$B$2*H5</f>
-        <v>-5752.5529570920671</v>
+        <v>-5646.5995563725201</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -2365,73 +2368,73 @@
       <c r="A7" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="53">
         <f>MIRR(E8:H8,B3,B3)</f>
-        <v>0.3041083591387852</v>
+        <v>0.29604808311628417</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="45">
         <v>0</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="46">
         <f>F5+F6</f>
-        <v>16203.645173502486</v>
-      </c>
-      <c r="G7" s="51">
+        <v>15904.70522147233</v>
+      </c>
+      <c r="G7" s="45">
         <f t="shared" ref="G7:H7" si="1">G5+G6</f>
-        <v>21640.556362393971</v>
-      </c>
-      <c r="H7" s="61">
+        <v>21241.969759687101</v>
+      </c>
+      <c r="H7" s="55">
         <f t="shared" si="1"/>
-        <v>21640.556362393971</v>
+        <v>21241.969759687101</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="50">
         <f>E2</f>
         <v>-29330.320372727783</v>
       </c>
       <c r="F8" s="3">
         <f>F7</f>
-        <v>16203.645173502486</v>
-      </c>
-      <c r="G8" s="56">
+        <v>15904.70522147233</v>
+      </c>
+      <c r="G8" s="50">
         <f>G7</f>
-        <v>21640.556362393971</v>
-      </c>
-      <c r="H8" s="57">
+        <v>21241.969759687101</v>
+      </c>
+      <c r="H8" s="51">
         <f>H7</f>
-        <v>21640.556362393971</v>
+        <v>21241.969759687101</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="52">
         <f>E8/(1+$B$2)^E1</f>
         <v>-29330.320372727783</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="48">
         <f>F8/(1+$B$2)^F1</f>
-        <v>13391.442292150816</v>
-      </c>
-      <c r="G9" s="58">
+        <v>13144.384480555645</v>
+      </c>
+      <c r="G9" s="52">
         <f>G8/(1+$B$2)^G1</f>
-        <v>14780.791177101271</v>
-      </c>
-      <c r="H9" s="55">
+        <v>14508.551164324228</v>
+      </c>
+      <c r="H9" s="49">
         <f>H8/(1+$B$2)^H1</f>
-        <v>12215.529898430803</v>
+        <v>11990.538152334073</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>

</xml_diff>

<commit_message>
Commit para que git deje de llorar
</commit_message>
<xml_diff>
--- a/Documentación/Factibilidad económica/Factibilidad económica.xlsx
+++ b/Documentación/Factibilidad económica/Factibilidad económica.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Costos" sheetId="1" r:id="rId1"/>
@@ -397,12 +397,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="[$USD]\ #,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -914,7 +915,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
@@ -988,33 +989,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1050,11 +1024,39 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
@@ -1341,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,10 +1353,10 @@
     <col min="2" max="2" width="40.109375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="27.5546875" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
@@ -1363,25 +1365,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="82"/>
+      <c r="E1" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
-      <c r="K1" s="53" t="s">
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+      <c r="K1" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="55"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="79"/>
       <c r="R1" t="s">
         <v>75</v>
       </c>
@@ -1438,7 +1440,7 @@
       <c r="B3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="74">
         <f>43.49</f>
         <v>43.49</v>
       </c>
@@ -1449,13 +1451,13 @@
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="86">
         <v>2.0541999999999998</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="83">
+      <c r="I3" s="87">
         <f t="shared" ref="I3:I17" si="0">H3*G3</f>
         <v>2.0541999999999998</v>
       </c>
@@ -1465,14 +1467,14 @@
       <c r="L3" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="M3" s="79">
+      <c r="M3" s="70">
         <f>13500/Q15</f>
         <v>16.520228101519862</v>
       </c>
       <c r="N3" s="44">
         <v>1</v>
       </c>
-      <c r="O3" s="81">
+      <c r="O3" s="72">
         <f>N3*M3</f>
         <v>16.520228101519862</v>
       </c>
@@ -1487,7 +1489,7 @@
       <c r="B4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="74">
         <f>19.94</f>
         <v>19.940000000000001</v>
       </c>
@@ -1498,13 +1500,13 @@
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="86">
         <v>0.13289999999999999</v>
       </c>
       <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="I4" s="83">
+      <c r="I4" s="87">
         <f t="shared" si="0"/>
         <v>0.26579999999999998</v>
       </c>
@@ -1514,14 +1516,14 @@
       <c r="L4" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="M4" s="79">
+      <c r="M4" s="70">
         <f>0.41</f>
         <v>0.41</v>
       </c>
       <c r="N4" s="44">
         <v>2</v>
       </c>
-      <c r="O4" s="81">
+      <c r="O4" s="72">
         <f t="shared" ref="O4:O21" si="1">N4*M4</f>
         <v>0.82</v>
       </c>
@@ -1533,7 +1535,7 @@
       <c r="B5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="74">
         <f>1250/Q6</f>
         <v>4.566443580676272</v>
       </c>
@@ -1544,13 +1546,13 @@
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="86">
         <v>5.5599999999999997E-2</v>
       </c>
       <c r="H5" s="4">
         <v>3</v>
       </c>
-      <c r="I5" s="83">
+      <c r="I5" s="87">
         <f t="shared" si="0"/>
         <v>0.1668</v>
       </c>
@@ -1560,14 +1562,14 @@
       <c r="L5" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="M5" s="79">
+      <c r="M5" s="70">
         <f>0.21</f>
         <v>0.21</v>
       </c>
       <c r="N5" s="44">
         <v>1</v>
       </c>
-      <c r="O5" s="81">
+      <c r="O5" s="72">
         <f t="shared" si="1"/>
         <v>0.21</v>
       </c>
@@ -1582,7 +1584,7 @@
       <c r="B6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="74">
         <f>13700/Q9</f>
         <v>39.42729692783653</v>
       </c>
@@ -1593,13 +1595,13 @@
       <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="86">
         <v>6.3E-2</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="83">
+      <c r="I6" s="87">
         <f t="shared" si="0"/>
         <v>6.3E-2</v>
       </c>
@@ -1609,14 +1611,14 @@
       <c r="L6" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="79">
+      <c r="M6" s="70">
         <f>0.01</f>
         <v>0.01</v>
       </c>
       <c r="N6" s="44">
         <v>3</v>
       </c>
-      <c r="O6" s="81">
+      <c r="O6" s="72">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
@@ -1631,7 +1633,7 @@
       <c r="B7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="74">
         <f>104.54</f>
         <v>104.54</v>
       </c>
@@ -1642,13 +1644,13 @@
       <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="86">
         <v>1.95E-2</v>
       </c>
       <c r="H7" s="4">
         <v>1</v>
       </c>
-      <c r="I7" s="83">
+      <c r="I7" s="87">
         <f t="shared" si="0"/>
         <v>1.95E-2</v>
       </c>
@@ -1658,14 +1660,14 @@
       <c r="L7" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="M7" s="79">
+      <c r="M7" s="70">
         <f>0.01</f>
         <v>0.01</v>
       </c>
       <c r="N7" s="44">
         <v>2</v>
       </c>
-      <c r="O7" s="81">
+      <c r="O7" s="72">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
@@ -1677,7 +1679,7 @@
       <c r="B8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="74">
         <f>19800/Q12</f>
         <v>57.096224440067708</v>
       </c>
@@ -1688,14 +1690,14 @@
       <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="66">
+      <c r="G8" s="86">
         <f>0.0471</f>
         <v>4.7100000000000003E-2</v>
       </c>
       <c r="H8" s="4">
         <v>1</v>
       </c>
-      <c r="I8" s="83">
+      <c r="I8" s="87">
         <f t="shared" si="0"/>
         <v>4.7100000000000003E-2</v>
       </c>
@@ -1705,14 +1707,14 @@
       <c r="L8" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="79">
+      <c r="M8" s="70">
         <f>0.01</f>
         <v>0.01</v>
       </c>
       <c r="N8" s="44">
         <v>2</v>
       </c>
-      <c r="O8" s="81">
+      <c r="O8" s="72">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
@@ -1727,7 +1729,7 @@
       <c r="B9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="74">
         <f>17290/Q12</f>
         <v>49.858268715594477</v>
       </c>
@@ -1738,14 +1740,14 @@
       <c r="F9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="66">
+      <c r="G9" s="86">
         <f>0.0073</f>
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="H9" s="6">
         <v>2</v>
       </c>
-      <c r="I9" s="83">
+      <c r="I9" s="87">
         <f t="shared" si="0"/>
         <v>1.46E-2</v>
       </c>
@@ -1755,14 +1757,14 @@
       <c r="L9" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="79">
+      <c r="M9" s="70">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="N9" s="44">
         <v>1</v>
       </c>
-      <c r="O9" s="81">
+      <c r="O9" s="72">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1777,7 +1779,7 @@
       <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="74">
         <f>4*4*236*7.5</f>
         <v>28320</v>
       </c>
@@ -1788,13 +1790,13 @@
       <c r="F10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="66">
+      <c r="G10" s="86">
         <v>1.12E-2</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="83">
+      <c r="I10" s="87">
         <f t="shared" si="0"/>
         <v>1.12E-2</v>
       </c>
@@ -1804,14 +1806,14 @@
       <c r="L10" s="49">
         <v>22013047</v>
       </c>
-      <c r="M10" s="79">
+      <c r="M10" s="70">
         <f>0.26</f>
         <v>0.26</v>
       </c>
       <c r="N10" s="44">
         <v>2</v>
       </c>
-      <c r="O10" s="81">
+      <c r="O10" s="72">
         <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
@@ -1823,7 +1825,7 @@
       <c r="B11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="74">
         <f>75000/Q15</f>
         <v>91.779045008443674</v>
       </c>
@@ -1834,13 +1836,13 @@
       <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="66">
+      <c r="G11" s="86">
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="H11" s="4">
         <v>1</v>
       </c>
-      <c r="I11" s="83">
+      <c r="I11" s="87">
         <f t="shared" si="0"/>
         <v>7.3000000000000001E-3</v>
       </c>
@@ -1850,14 +1852,14 @@
       <c r="L11" s="49">
         <v>22232041</v>
       </c>
-      <c r="M11" s="79">
+      <c r="M11" s="70">
         <f>0.45</f>
         <v>0.45</v>
       </c>
       <c r="N11" s="44">
         <v>2</v>
       </c>
-      <c r="O11" s="81">
+      <c r="O11" s="72">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
@@ -1872,7 +1874,7 @@
       <c r="B12" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="86">
+      <c r="C12" s="75">
         <f>490000/Q15</f>
         <v>599.62309405516532</v>
       </c>
@@ -1882,14 +1884,14 @@
       <c r="F12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="66">
+      <c r="G12" s="86">
         <v>0.16028000000000001</v>
       </c>
       <c r="H12" s="7">
         <f>4</f>
         <v>4</v>
       </c>
-      <c r="I12" s="83">
+      <c r="I12" s="87">
         <f t="shared" si="0"/>
         <v>0.64112000000000002</v>
       </c>
@@ -1899,14 +1901,14 @@
       <c r="L12" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="M12" s="79">
+      <c r="M12" s="70">
         <f>0.27</f>
         <v>0.27</v>
       </c>
       <c r="N12" s="44">
         <v>2</v>
       </c>
-      <c r="O12" s="81">
+      <c r="O12" s="72">
         <f t="shared" si="1"/>
         <v>0.54</v>
       </c>
@@ -1919,7 +1921,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="27"/>
-      <c r="C13" s="87">
+      <c r="C13" s="76">
         <f>SUM(C3:C12)</f>
         <v>29330.320372727783</v>
       </c>
@@ -1929,14 +1931,14 @@
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="66">
+      <c r="G13" s="86">
         <f>589/Q15</f>
         <v>0.72077143346631101</v>
       </c>
       <c r="H13" s="6">
         <v>2</v>
       </c>
-      <c r="I13" s="83">
+      <c r="I13" s="87">
         <f t="shared" si="0"/>
         <v>1.441542866932622</v>
       </c>
@@ -1946,14 +1948,14 @@
       <c r="L13" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="79">
+      <c r="M13" s="70">
         <f>19.8</f>
         <v>19.8</v>
       </c>
       <c r="N13" s="48">
         <v>0.2</v>
       </c>
-      <c r="O13" s="81">
+      <c r="O13" s="72">
         <f>N13*M13</f>
         <v>3.9600000000000004</v>
       </c>
@@ -1965,7 +1967,7 @@
       <c r="F14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="66">
+      <c r="G14" s="86">
         <f>89000/Q15</f>
         <v>108.91113341001983</v>
       </c>
@@ -1973,7 +1975,7 @@
         <f>3/750</f>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I14" s="83">
+      <c r="I14" s="87">
         <f t="shared" si="0"/>
         <v>0.43564453364007932</v>
       </c>
@@ -1983,14 +1985,14 @@
       <c r="L14" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="M14" s="80">
+      <c r="M14" s="71">
         <f>(12167/40)/Q15</f>
         <v>0.37222521353924476</v>
       </c>
       <c r="N14" s="44">
         <v>1</v>
       </c>
-      <c r="O14" s="81">
+      <c r="O14" s="72">
         <f t="shared" si="1"/>
         <v>0.37222521353924476</v>
       </c>
@@ -2005,14 +2007,14 @@
       <c r="F15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="66">
+      <c r="G15" s="86">
         <f>27.55</f>
         <v>27.55</v>
       </c>
       <c r="H15" s="8">
         <v>0.01</v>
       </c>
-      <c r="I15" s="83">
+      <c r="I15" s="87">
         <f t="shared" si="0"/>
         <v>0.27550000000000002</v>
       </c>
@@ -2022,14 +2024,14 @@
       <c r="L15" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="M15" s="80">
+      <c r="M15" s="71">
         <f>1560/Q15</f>
         <v>1.9090041361756285</v>
       </c>
       <c r="N15" s="44">
         <v>4</v>
       </c>
-      <c r="O15" s="81">
+      <c r="O15" s="72">
         <f t="shared" si="1"/>
         <v>7.6360165447025139</v>
       </c>
@@ -2044,14 +2046,14 @@
       <c r="F16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="66">
+      <c r="G16" s="86">
         <f>7.5</f>
         <v>7.5</v>
       </c>
       <c r="H16" s="17">
         <v>0.5</v>
       </c>
-      <c r="I16" s="83">
+      <c r="I16" s="87">
         <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
@@ -2061,14 +2063,14 @@
       <c r="L16" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="M16" s="79">
+      <c r="M16" s="70">
         <f>2760/Q15</f>
         <v>3.3774688563107271</v>
       </c>
       <c r="N16" s="44">
         <v>1</v>
       </c>
-      <c r="O16" s="81">
+      <c r="O16" s="72">
         <f t="shared" si="1"/>
         <v>3.3774688563107271</v>
       </c>
@@ -2080,14 +2082,14 @@
       <c r="F17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="66">
+      <c r="G17" s="86">
         <f>7.5</f>
         <v>7.5</v>
       </c>
       <c r="H17" s="6">
         <v>0.5</v>
       </c>
-      <c r="I17" s="83">
+      <c r="I17" s="87">
         <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
@@ -2097,14 +2099,14 @@
       <c r="L17" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="M17" s="79">
+      <c r="M17" s="70">
         <f>(15444/20)/Q15</f>
         <v>0.9449570474069362</v>
       </c>
       <c r="N17" s="44">
         <v>2</v>
       </c>
-      <c r="O17" s="81">
+      <c r="O17" s="72">
         <f t="shared" si="1"/>
         <v>1.8899140948138724</v>
       </c>
@@ -2116,7 +2118,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="84">
+      <c r="I18" s="88">
         <f>SUM(I3:I17)</f>
         <v>12.943307400572701</v>
       </c>
@@ -2126,14 +2128,14 @@
       <c r="L18" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="M18" s="79">
+      <c r="M18" s="70">
         <f>(5251/10)/Q15</f>
         <v>0.64257568711911706</v>
       </c>
       <c r="N18" s="44">
         <v>2</v>
       </c>
-      <c r="O18" s="81">
+      <c r="O18" s="72">
         <f t="shared" si="1"/>
         <v>1.2851513742382341</v>
       </c>
@@ -2145,14 +2147,14 @@
       <c r="L19" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="M19" s="79">
+      <c r="M19" s="70">
         <f>(1691/50)/Q15</f>
         <v>4.1386230695807533E-2</v>
       </c>
       <c r="N19" s="44">
         <v>2</v>
       </c>
-      <c r="O19" s="81">
+      <c r="O19" s="72">
         <f t="shared" si="1"/>
         <v>8.2772461391615065E-2</v>
       </c>
@@ -2164,14 +2166,14 @@
       <c r="L20" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="M20" s="79">
+      <c r="M20" s="70">
         <f>16200/Q15</f>
         <v>19.824273721823836</v>
       </c>
       <c r="N20" s="44">
         <v>0.04</v>
       </c>
-      <c r="O20" s="81">
+      <c r="O20" s="72">
         <f t="shared" si="1"/>
         <v>0.7929709488729535</v>
       </c>
@@ -2183,14 +2185,14 @@
       <c r="L21" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="M21" s="79">
+      <c r="M21" s="70">
         <f>7.5</f>
         <v>7.5</v>
       </c>
       <c r="N21" s="44">
         <v>2</v>
       </c>
-      <c r="O21" s="81">
+      <c r="O21" s="72">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -2202,7 +2204,7 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="82">
+      <c r="O22" s="73">
         <f>SUM(O3:O21)</f>
         <v>54.976747595389028</v>
       </c>
@@ -2244,12 +2246,12 @@
       <c r="A1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="85"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2298,15 +2300,15 @@
       <c r="D4" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="68">
         <f>E3*$B$3</f>
         <v>26250</v>
       </c>
-      <c r="F4" s="77">
+      <c r="F4" s="68">
         <f>F3*$B$3</f>
         <v>35000</v>
       </c>
-      <c r="G4" s="78">
+      <c r="G4" s="69">
         <f>G3*$B$3</f>
         <v>35000</v>
       </c>
@@ -2316,12 +2318,12 @@
       <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2371,15 +2373,15 @@
       <c r="D9" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="68">
         <f>E8*$B$8</f>
         <v>800</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="68">
         <f t="shared" ref="F9" si="0">F8*$B$8</f>
         <v>1120</v>
       </c>
-      <c r="G9" s="78">
+      <c r="G9" s="69">
         <f>G8*$B$8</f>
         <v>1120</v>
       </c>
@@ -2414,7 +2416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2457,17 +2459,17 @@
       <c r="D2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="76">
+      <c r="E2" s="67">
         <f>-Costos!C13</f>
         <v>-29330.320372727783</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="55" t="s">
         <v>117</v>
       </c>
       <c r="I2" s="39"/>
@@ -2477,24 +2479,24 @@
       <c r="A3" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="63">
+      <c r="B3" s="54">
         <v>0.152</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="66">
+      <c r="F3" s="57">
         <f>Ingresos!E4+Ingresos!E9</f>
         <v>27050</v>
       </c>
-      <c r="G3" s="65">
+      <c r="G3" s="56">
         <f>Ingresos!F4+Ingresos!F9</f>
         <v>36120</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="58">
         <f>Ingresos!G4+Ingresos!G9</f>
         <v>36120</v>
       </c>
@@ -2505,18 +2507,18 @@
       <c r="D4" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="66">
+      <c r="F4" s="57">
         <f>-Ingresos!E3*Costos!$I$18 - Ingresos!F8*Costos!$O$22</f>
         <v>-7564.9108516361148</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="56">
         <f>-Ingresos!F3*Costos!$I$18 - Ingresos!F8*Costos!$O$22</f>
         <v>-9829.989646736336</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="59">
         <f>-Ingresos!G3*Costos!$I$18 - Ingresos!G8*Costos!$O$22</f>
         <v>-9829.989646736336</v>
       </c>
@@ -2534,18 +2536,18 @@
       <c r="D5" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="66">
+      <c r="F5" s="57">
         <f>F3+F4</f>
         <v>19485.089148363884</v>
       </c>
-      <c r="G5" s="65">
+      <c r="G5" s="56">
         <f t="shared" ref="G5:H5" si="0">G3+G4</f>
         <v>26290.010353263664</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="58">
         <f t="shared" si="0"/>
         <v>26290.010353263664</v>
       </c>
@@ -2563,18 +2565,18 @@
       <c r="D6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="F6" s="66">
+      <c r="F6" s="57">
         <f>-$B$2*F5</f>
         <v>-5845.5267445091649</v>
       </c>
-      <c r="G6" s="65">
+      <c r="G6" s="56">
         <f>-$B$2*G5</f>
         <v>-7887.003105979099</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="58">
         <f>-$B$2*H5</f>
         <v>-7887.003105979099</v>
       </c>
@@ -2592,18 +2594,18 @@
       <c r="D7" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="61">
         <f>F5+F6</f>
         <v>13639.562403854719</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="60">
         <f>G5+G6</f>
         <v>18403.007247284564</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="62">
         <f>H5+H6</f>
         <v>18403.007247284564</v>
       </c>
@@ -2611,22 +2613,22 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="63">
         <f>E2</f>
         <v>-29330.320372727783</v>
       </c>
-      <c r="F8" s="66">
+      <c r="F8" s="57">
         <f>F7</f>
         <v>13639.562403854719</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="63">
         <f>G7</f>
         <v>18403.007247284564</v>
       </c>
-      <c r="H8" s="67">
+      <c r="H8" s="58">
         <f>H7</f>
         <v>18403.007247284564</v>
       </c>
@@ -2637,19 +2639,19 @@
       <c r="D9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="64">
         <f>E8/(1+$B$3)^E1</f>
         <v>-29330.320372727783</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="64">
         <f>F8/(1+$B$3)^F1</f>
         <v>11839.897920012778</v>
       </c>
-      <c r="G9" s="73">
+      <c r="G9" s="64">
         <f>G8/(1+$B$3)^G1</f>
         <v>13867.042256887604</v>
       </c>
-      <c r="H9" s="74">
+      <c r="H9" s="65">
         <f>H8/(1+$B$3)^H1</f>
         <v>12037.363070214935</v>
       </c>

</xml_diff>